<commit_message>
Final Draft of the report (To be checked a final time)
</commit_message>
<xml_diff>
--- a/Data/Graphs & Data for Key Insites.xlsx
+++ b/Data/Graphs & Data for Key Insites.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Reason for Recalls Chart" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Normalized Values for Fragments" sheetId="8" r:id="rId8"/>
     <sheet name="Meat Recall Chart" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1250,8 +1250,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Types of Food Poisning</a:t>
+              <a:t>Types of Food </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Poisoning</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2039,6 +2046,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-BC70-40A8-94F8-92910D91C26B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -2054,6 +2066,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-BC70-40A8-94F8-92910D91C26B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -2069,6 +2086,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-BC70-40A8-94F8-92910D91C26B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -2084,6 +2106,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-BC70-40A8-94F8-92910D91C26B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -2099,6 +2126,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-BC70-40A8-94F8-92910D91C26B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -2114,6 +2146,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-BC70-40A8-94F8-92910D91C26B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -2433,6 +2470,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-3DF4-4A25-B4ED-8AC8B3B1642E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -2448,6 +2490,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-3DF4-4A25-B4ED-8AC8B3B1642E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -2483,6 +2530,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-3DF4-4A25-B4ED-8AC8B3B1642E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -2500,6 +2552,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-3DF4-4A25-B4ED-8AC8B3B1642E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -2517,6 +2574,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-3DF4-4A25-B4ED-8AC8B3B1642E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -2534,6 +2596,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-3DF4-4A25-B4ED-8AC8B3B1642E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -2551,6 +2618,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-3DF4-4A25-B4ED-8AC8B3B1642E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -6359,16 +6431,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1571625</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6395,16 +6467,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>347664</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>595314</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7054,7 +7126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F16" sqref="F15:F16"/>
     </sheetView>
   </sheetViews>
@@ -7127,11 +7199,12 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9229,8 +9302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>